<commit_message>
Se crea una nueva rama
</commit_message>
<xml_diff>
--- a/datos/Data.xlsx
+++ b/datos/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sqasa1-my.sharepoint.com/personal/joan_bonilla_sqasa_co/Documents/Escritorio/ProyectoBanco/datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancodebogota-my.sharepoint.com/personal/jboni18_bancodebogota_com_co/Documents/Documentos/ProyectoBB1/PruebasAbc/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_AD4D2F04E46CFB4ACB3E20EB0DD0C5A8693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{474DD5B4-0ED2-40EC-96B0-B1E1F1CF6920}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4D2F04E46CFB4ACB3E20EB0DD0C5A8693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E0991F5-C833-43EF-8DD3-02B34973C149}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="480" windowWidth="20460" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuentas" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -370,7 +373,7 @@
       <c r="A2" s="1">
         <v>1006</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>100</v>
       </c>
     </row>
@@ -378,7 +381,7 @@
       <c r="A3" s="1">
         <v>1005</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>200</v>
       </c>
     </row>
@@ -386,7 +389,7 @@
       <c r="A4" s="1">
         <v>1004</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>300</v>
       </c>
     </row>

</xml_diff>